<commit_message>
adjusted the query keys
</commit_message>
<xml_diff>
--- a/exploration/queries_guidlines_draft.xlsx
+++ b/exploration/queries_guidlines_draft.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/zxowg46_s-cloud_uni-tuebingen_de/Documents/Thesis/esg_extraction/exploration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28732819-E715-4221-8FC4-9049E8397DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{28732819-E715-4221-8FC4-9049E8397DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8DE16F5-14BB-423A-88DA-2CF95D3D482C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{42EA4C40-D73F-43B7-B155-9FD3BB8C40D8}"/>
   </bookViews>
@@ -356,9 +356,6 @@
     <t>Does the company state whether its policies related to its own workforce explicitly address trafficking in human beings, forced labour or compulsory labour, and child labour?</t>
   </si>
   <si>
-    <t>S1_C12</t>
-  </si>
-  <si>
     <t>Does the company explain the existence and role of any Global Framework Agreement or other agreements with workers’ representatives related to respecting the human rights of its own workforce?</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>AR 20</t>
   </si>
   <si>
-    <t>S1_C13</t>
-  </si>
-  <si>
     <t>Does the company disclose the number of severe human rights incidents connected to its workforce during the reporting period?</t>
   </si>
   <si>
@@ -386,9 +380,6 @@
     <t>AR 103-AR 106</t>
   </si>
   <si>
-    <t>S1_C14</t>
-  </si>
-  <si>
     <t>Does the company disclose the total amount of fines, penalties, and compensation paid related to the severe human rights incidents connected to its workforce?</t>
   </si>
   <si>
@@ -780,6 +771,15 @@
   </si>
   <si>
     <t>If not all employees are covered by social protection, does the company disclose the countries where gaps in social protection exist?</t>
+  </si>
+  <si>
+    <t>S1_C1</t>
+  </si>
+  <si>
+    <t>S1_C2</t>
+  </si>
+  <si>
+    <t>S1_C3</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD330E28-43DB-449D-9BDC-121D276E2900}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C19" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1816,7 +1816,7 @@
         <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>245</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>84</v>
@@ -1836,7 +1836,7 @@
         <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>246</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>87</v>
@@ -1856,7 +1856,7 @@
         <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>247</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>90</v>
@@ -1876,7 +1876,7 @@
         <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>93</v>
@@ -1896,7 +1896,7 @@
         <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>96</v>
@@ -1916,7 +1916,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>99</v>
@@ -1937,7 +1937,7 @@
         <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>102</v>
@@ -1960,7 +1960,7 @@
         <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>105</v>
@@ -1981,10 +1981,10 @@
         <v>82</v>
       </c>
       <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>22</v>
@@ -1993,10 +1993,10 @@
         <v>37</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
@@ -2004,22 +2004,22 @@
         <v>82</v>
       </c>
       <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="G31" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
@@ -2027,33 +2027,33 @@
         <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>22</v>
@@ -2062,182 +2062,182 @@
         <v>37</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F34" s="4">
         <v>27</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="G36" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="G39" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F41" s="3">
         <v>28</v>
@@ -2246,76 +2246,76 @@
     </row>
     <row r="42" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="F42" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>22</v>
@@ -2324,42 +2324,42 @@
         <v>37</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>22</v>
@@ -2368,429 +2368,429 @@
         <v>37</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E49" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B50" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="G51" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="G52" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B55" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="G55" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F57" s="4">
         <v>33</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B58" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F58" s="4">
         <v>33</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F59" s="4">
         <v>33</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B61" t="s">
+      <c r="F61" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="G61" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" t="s">
+        <v>231</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="F62" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
+        <v>225</v>
+      </c>
+      <c r="B63" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B63" t="s">
-        <v>237</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="F63" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
+        <v>225</v>
+      </c>
+      <c r="B64" t="s">
+        <v>237</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B64" t="s">
-        <v>240</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="F64" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
+        <v>225</v>
+      </c>
+      <c r="B65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B65" t="s">
-        <v>243</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="F65" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>225</v>
+      </c>
+      <c r="B66" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="B66" t="s">
-        <v>246</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="F66" s="4">
         <v>75</v>

</xml_diff>